<commit_message>
Finalizada versão 0.1 do sistema GTI-Competências
</commit_message>
<xml_diff>
--- a/output/xlsx/RF006 - Gerenciar Perfis de Competências--GT-.xlsx
+++ b/output/xlsx/RF006 - Gerenciar Perfis de Competências--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="66">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -41,13 +41,13 @@
     <t>Reduced (Greedy Heuristic - Transition Coverage)</t>
   </si>
   <si>
-    <t>Size: 6 test case(s))</t>
+    <t>Size: 7 test case(s))</t>
   </si>
   <si>
     <t xml:space="preserve">Creation Date: </t>
   </si>
   <si>
-    <t>13/04/2024</t>
+    <t>15/04/2024</t>
   </si>
   <si>
     <t xml:space="preserve">Test Case ID: </t>
@@ -185,22 +185,31 @@
     <t>TC4</t>
   </si>
   <si>
+    <t>Usuario Não-Autenticado acessa a funcionalidade de gestão de perfis de competências a partir do menu inicial</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe a listagem dos perfis de competências cadastrados apenas para visualização com a opção 'Ajuda'</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
     <t>Líder de Pessoas clica na opção 'Novo' para criar um novo perfil</t>
   </si>
   <si>
     <t>SYSTEM exibe uma mensagem de erro ao tentar salvar o novo perfil, informando o campo ou a validação que falhou</t>
   </si>
   <si>
-    <t>TC5</t>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe uma mensagem de erro ao tentar editar o perfil, informando o campo ou a validação que falhou</t>
+  </si>
+  <si>
+    <t>TC7</t>
   </si>
   <si>
     <t>SYSTEM exibe uma mensagem de erro ao tentar excluir o perfil</t>
-  </si>
-  <si>
-    <t>TC6</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe uma mensagem de erro ao tentar editar o perfil, informando o campo ou a validação que falhou</t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -1183,13 +1192,13 @@
         <v>1.0</v>
       </c>
       <c r="B47" t="s" s="7">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D47" t="s" s="7">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E47" t="s" s="6">
         <v>2</v>
@@ -1198,138 +1207,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B48" t="s" s="7">
-        <v>57</v>
-      </c>
-      <c r="C48" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D48" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="E48" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F48" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B49" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C49" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="E49" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F49" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="48"/>
+    <row r="49"/>
     <row r="50">
-      <c r="A50" t="n" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="B50" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C50" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E50" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F50" t="s" s="6">
+      <c r="A50" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B50" t="s" s="4">
+        <v>59</v>
+      </c>
+      <c r="C50" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D50" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B51" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C51" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E51" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F51" t="s" s="6">
+      <c r="A51" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B51" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F51" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B52" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="C52" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E52" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F52" t="s" s="6">
+      <c r="A52" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B52" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B53" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="C53" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D53" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="E53" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F53" t="s" s="6">
-        <v>2</v>
+      <c r="A53" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C53" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D53" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E53" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F53" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n" s="10">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="B54" t="s" s="7">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C54" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D54" t="s" s="7">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E54" t="s" s="6">
         <v>2</v>
@@ -1340,16 +1311,16 @@
     </row>
     <row r="55">
       <c r="A55" t="n" s="10">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
       <c r="B55" t="s" s="7">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D55" t="s" s="7">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="E55" t="s" s="6">
         <v>2</v>
@@ -1358,100 +1329,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56"/>
-    <row r="57"/>
+    <row r="56">
+      <c r="A56" t="n" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="B56" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C56" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E56" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B57" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C57" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E57" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F57" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="58">
-      <c r="A58" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B58" t="s" s="4">
-        <v>59</v>
-      </c>
-      <c r="C58" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D58" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E58" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F58" t="s" s="4">
+      <c r="A58" t="n" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B58" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C58" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D58" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E58" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F58" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B59" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C59" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F59" t="s" s="9">
+      <c r="A59" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B59" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C59" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E59" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F59" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B60" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C60" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E60" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F60" t="s" s="8">
+      <c r="A60" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B60" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C60" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E60" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F60" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B61" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C61" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D61" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E61" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F61" t="s" s="5">
-        <v>25</v>
+      <c r="A61" t="n" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="B61" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="C61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n" s="10">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="B62" t="s" s="7">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C62" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D62" t="s" s="7">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="E62" t="s" s="6">
         <v>2</v>
@@ -1460,138 +1469,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B63" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="C63" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D63" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="E63" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F63" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B64" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="C64" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="E64" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F64" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="63"/>
+    <row r="64"/>
     <row r="65">
-      <c r="A65" t="n" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="B65" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C65" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="E65" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F65" t="s" s="6">
+      <c r="A65" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="C65" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D65" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F65" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B66" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C66" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D66" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E66" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F66" t="s" s="6">
+      <c r="A66" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F66" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B67" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C67" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D67" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E67" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F67" t="s" s="6">
+      <c r="A67" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B67" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C67" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F67" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B68" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="C68" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D68" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E68" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F68" t="s" s="6">
-        <v>2</v>
+      <c r="A68" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C68" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D68" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E68" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F68" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n" s="10">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1602,16 +1573,16 @@
     </row>
     <row r="70">
       <c r="A70" t="n" s="10">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
       <c r="B70" t="s" s="7">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C70" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E70" t="s" s="6">
         <v>2</v>
@@ -1622,16 +1593,16 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
       <c r="B71" t="s" s="7">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C71" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="E71" t="s" s="6">
         <v>2</v>
@@ -1640,100 +1611,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72"/>
-    <row r="73"/>
+    <row r="72">
+      <c r="A72" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B72" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C72" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E72" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F72" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B73" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C73" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E73" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F73" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="74">
-      <c r="A74" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B74" t="s" s="4">
-        <v>61</v>
-      </c>
-      <c r="C74" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D74" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E74" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F74" t="s" s="4">
+      <c r="A74" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B74" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C74" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E74" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F74" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B75" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C75" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D75" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E75" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F75" t="s" s="9">
+      <c r="A75" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B75" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C75" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E75" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F75" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B76" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C76" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D76" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E76" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F76" t="s" s="8">
+      <c r="A76" t="n" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="B76" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C76" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E76" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F76" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B77" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C77" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D77" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E77" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F77" t="s" s="5">
-        <v>25</v>
+      <c r="A77" t="n" s="10">
+        <v>9.0</v>
+      </c>
+      <c r="B77" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="C77" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E77" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F77" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n" s="10">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="B78" t="s" s="7">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C78" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D78" t="s" s="7">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="E78" t="s" s="6">
         <v>2</v>
@@ -1742,138 +1751,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B79" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="C79" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D79" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="E79" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F79" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B80" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="C80" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D80" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="E80" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F80" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="79"/>
+    <row r="80"/>
     <row r="81">
-      <c r="A81" t="n" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="B81" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C81" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D81" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="E81" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F81" t="s" s="6">
+      <c r="A81" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B81" t="s" s="4">
+        <v>64</v>
+      </c>
+      <c r="C81" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D81" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E81" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F81" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B82" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C82" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E82" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F82" t="s" s="6">
+      <c r="A82" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B82" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F82" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B83" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C83" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E83" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F83" t="s" s="6">
+      <c r="A83" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B83" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C83" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E83" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F83" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B84" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="C84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s" s="6">
-        <v>2</v>
+      <c r="A84" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C84" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D84" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E84" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F84" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n" s="10">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="B85" t="s" s="7">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C85" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D85" t="s" s="7">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E85" t="s" s="6">
         <v>2</v>
@@ -1884,16 +1855,16 @@
     </row>
     <row r="86">
       <c r="A86" t="n" s="10">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C86" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E86" t="s" s="6">
         <v>2</v>
@@ -1904,21 +1875,161 @@
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="B87" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="C87" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D87" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="E87" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F87" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B88" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C88" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E88" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F88" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B89" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C89" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E89" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F89" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B90" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C90" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E90" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F90" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B91" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C91" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D91" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E91" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F91" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="B92" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C92" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E92" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F92" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n" s="10">
+        <v>9.0</v>
+      </c>
+      <c r="B93" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="C93" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E93" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F93" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n" s="10">
         <v>10.0</v>
       </c>
-      <c r="B87" t="s" s="7">
+      <c r="B94" t="s" s="7">
         <v>44</v>
       </c>
-      <c r="C87" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D87" t="s" s="7">
-        <v>62</v>
-      </c>
-      <c r="E87" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F87" t="s" s="6">
+      <c r="C94" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="E94" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F94" t="s" s="6">
         <v>2</v>
       </c>
     </row>
@@ -1934,10 +2045,12 @@
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:F83"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>